<commit_message>
Finalizar el sistema binario de cines y la serializacion
</commit_message>
<xml_diff>
--- a/src/binarios/binarios.xlsx
+++ b/src/binarios/binarios.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="formato de nuestro sistema" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>UTF-8</t>
   </si>
@@ -144,13 +145,97 @@
   </si>
   <si>
     <t>Pepe</t>
+  </si>
+  <si>
+    <t>registro</t>
+  </si>
+  <si>
+    <t>Multiples Registros</t>
+  </si>
+  <si>
+    <t>1 registro</t>
+  </si>
+  <si>
+    <t>1 dato</t>
+  </si>
+  <si>
+    <t>String rate</t>
+  </si>
+  <si>
+    <t>String tipo</t>
+  </si>
+  <si>
+    <t>boolean activa</t>
+  </si>
+  <si>
+    <t>int cod pelicula</t>
+  </si>
+  <si>
+    <t>int cod sala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int cod ticket </t>
+  </si>
+  <si>
+    <t>double precio</t>
+  </si>
+  <si>
+    <t>int cod peli</t>
+  </si>
+  <si>
+    <t>String horario</t>
+  </si>
+  <si>
+    <t>int cant asientos</t>
+  </si>
+  <si>
+    <t>*boolean asientos</t>
+  </si>
+  <si>
+    <t>cod peli</t>
+  </si>
+  <si>
+    <t>cod sala</t>
+  </si>
+  <si>
+    <t>cod ticket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">long fecha </t>
+  </si>
+  <si>
+    <t>long fecha</t>
+  </si>
+  <si>
+    <t>rp</t>
+  </si>
+  <si>
+    <t>rt</t>
+  </si>
+  <si>
+    <t>peliculas.cnk</t>
+  </si>
+  <si>
+    <t>codigos.cnk</t>
+  </si>
+  <si>
+    <t>sala+codsala.cnk</t>
+  </si>
+  <si>
+    <t>tickets.cnk</t>
+  </si>
+  <si>
+    <t>double duracion</t>
+  </si>
+  <si>
+    <t>xxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +245,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -199,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -271,11 +364,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -298,6 +413,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,15 +444,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>456239</xdr:colOff>
+      <xdr:colOff>452236</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>8001</xdr:rowOff>
+      <xdr:rowOff>168082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>16008</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>44020</xdr:rowOff>
+      <xdr:colOff>12005</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>12000</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -337,7 +461,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2737436" y="392203"/>
+          <a:off x="2733433" y="552284"/>
           <a:ext cx="320169" cy="420220"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -630,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,9 +986,197 @@
         <v>38</v>
       </c>
     </row>
+    <row r="27" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="E28" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="F28" s="17"/>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="19"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="19"/>
+    </row>
+    <row r="30" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="21"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="16">
+        <v>6</v>
+      </c>
+      <c r="C33" s="17"/>
+    </row>
+    <row r="34" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="20"/>
+      <c r="C34" s="21"/>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="23"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:H10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="286" zoomScaleNormal="286" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="3.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="1.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>